<commit_message>
adding charge / mass balance checking function
</commit_message>
<xml_diff>
--- a/tests/fixtures/min_model.xlsx
+++ b/tests/fixtures/min_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -50,6 +50,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Model!$A$1:$B$8</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Model!$A$1:$B$8</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Model!$A$1:$B$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Model!$A$1:$B$8</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
@@ -58,6 +59,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$H$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Submodels!$A$1:$H$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Submodels!$A$1:$H$2</definedName>
@@ -66,6 +68,7 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Submodels!$A$1:$H$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Submodels!$A$1:$H$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Submodels!$A$1:$H$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Submodels!$A$1:$H$2</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
@@ -74,6 +77,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$18</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$18</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$18</definedName>
@@ -82,6 +86,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$18</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$18</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$18</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$E$18</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">Concentrations!$A$1:$E$18</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Concentrations!$A$1:$E$18</definedName>
@@ -90,6 +95,7 @@
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Concentrations!$A$1:$E$18</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Concentrations!$A$1:$E$18</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Concentrations!$A$1:$E$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Concentrations!$A$1:$E$18</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Observables!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">Observables!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Observables!$A$1:$E$1</definedName>
@@ -98,6 +104,7 @@
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Observables!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Observables!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Observables!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Observables!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">Functions!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0" vbProcedure="false">Functions!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Functions!$A$1:$D$1</definedName>
@@ -106,6 +113,7 @@
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Functions!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Functions!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Functions!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Functions!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$I$6</definedName>
@@ -114,6 +122,7 @@
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
@@ -122,6 +131,7 @@
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
@@ -130,6 +140,7 @@
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
@@ -138,6 +149,7 @@
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$H$3</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$H$3</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$H$3</definedName>
@@ -146,6 +158,7 @@
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$H$3</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$H$3</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$H$3</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
@@ -154,6 +167,7 @@
     <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$Q$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$Q$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">References!$A$1:$Q$1</definedName>
@@ -162,6 +176,7 @@
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">References!$A$1:$Q$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$Q$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$Q$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$Q$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
@@ -170,6 +185,7 @@
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -874,7 +890,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="F8:F12 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -961,14 +977,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B10" activeCellId="1" sqref="F8:F12 B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.3481781376518"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1200,7 +1216,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="F8:F12 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1256,7 +1272,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="F8:F12 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1306,7 +1322,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H14" activeCellId="0" sqref="H14"/>
+      <selection pane="bottomRight" activeCell="H14" activeCellId="1" sqref="F8:F12 H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1397,7 +1413,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="F8:F12 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1444,7 +1460,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="F8:F12 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1530,7 +1546,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="F8:F12 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1595,7 +1611,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="F8:F12 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1653,12 +1669,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="1" sqref="F8:F12 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1740,7 +1756,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="F8:F12 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1811,21 +1827,21 @@
   </sheetPr>
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="F8" activeCellId="0" sqref="F8:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.17004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.4939271255061"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.9959514170041"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1868,9 +1884,11 @@
         <v>32</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>12.0107</v>
-      </c>
-      <c r="F2" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="G2" s="2" t="s">
         <v>33</v>
       </c>
@@ -1887,10 +1905,10 @@
         <v>35</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>1.008</v>
+        <v>1</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>33</v>
@@ -1908,9 +1926,11 @@
         <v>37</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>14.0067</v>
-      </c>
-      <c r="F4" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="G4" s="2" t="s">
         <v>33</v>
       </c>
@@ -1927,9 +1947,11 @@
         <v>39</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>15.9994</v>
-      </c>
-      <c r="F5" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="G5" s="2" t="s">
         <v>33</v>
       </c>
@@ -1946,10 +1968,10 @@
         <v>41</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>30.974</v>
+        <v>1</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>33</v>
@@ -1970,7 +1992,7 @@
         <v>174.949</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>33</v>
@@ -2012,7 +2034,7 @@
         <v>503.149</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>33</v>
@@ -2033,7 +2055,7 @@
         <v>479.123</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>33</v>
@@ -2054,7 +2076,7 @@
         <v>519.148</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>33</v>
@@ -2075,7 +2097,7 @@
         <v>480.107</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>33</v>
@@ -2095,10 +2117,10 @@
         <v>55</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>15992.1890999</v>
+        <v>1498</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>-51</v>
+        <v>-50</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>56</v>
@@ -2118,10 +2140,10 @@
         <v>58</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>15992.1890999</v>
+        <v>1818</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>-51</v>
+        <v>-76</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>56</v>
@@ -2141,10 +2163,10 @@
         <v>61</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>178432.010432886</v>
+        <v>2138</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>-56</v>
+        <v>-108</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>56</v>
@@ -2164,10 +2186,10 @@
         <v>63</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>178432.010432886</v>
+        <v>2458</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>-58</v>
+        <v>-120</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>56</v>
@@ -2187,10 +2209,10 @@
         <v>65</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>178432.010432886</v>
+        <v>2778</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>-55</v>
+        <v>-176</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>56</v>
@@ -2218,17 +2240,17 @@
   </sheetPr>
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="B10" activeCellId="1" sqref="F8:F12 B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2495,7 +2517,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="F8:F12 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2545,7 +2567,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="F8:F12 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2588,19 +2610,19 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="D21" activeCellId="1" sqref="F8:F12 D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.0607287449393"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.4898785425101"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.1012145748988"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="83.3400809716599"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.3157894736842"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="84.0890688259109"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
add compartments to submodels, which are now needed; fix tiny spelling mistake
</commit_message>
<xml_diff>
--- a/tests/fixtures/min_model.xlsx
+++ b/tests/fixtures/min_model.xlsx
@@ -8,9 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_test/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="989" activeTab="6"/>
+    <workbookView xWindow="-40920" yWindow="19260" windowWidth="22820" windowHeight="12320" tabRatio="989" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -176,7 +175,7 @@
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="2">Submodels!$A$1:$H$2</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="1">Taxon!$A$1:$A$5</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -192,7 +191,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="143">
   <si>
     <t>Id</t>
   </si>
@@ -1033,7 +1032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView windowProtection="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1107,14 +1106,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView windowProtection="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" activeCellId="1" sqref="F8:F12 B10"/>
+      <selection pane="bottomRight" activeCell="B10" activeCellId="1" sqref="F8:F12 A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1234,7 +1242,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="42" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>103</v>
       </c>
@@ -1251,7 +1259,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="42" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>105</v>
       </c>
@@ -1268,7 +1276,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="42" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>107</v>
       </c>
@@ -1285,7 +1293,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="42" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>109</v>
       </c>
@@ -1302,7 +1310,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="42" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>111</v>
       </c>
@@ -1330,7 +1338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView windowProtection="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1373,7 +1381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView windowProtection="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1410,7 +1418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView windowProtection="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1488,7 +1496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView windowProtection="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1522,7 +1530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView windowProtection="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1595,7 +1603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView windowProtection="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1647,7 +1655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView windowProtection="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1692,14 +1700,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView windowProtection="1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="1" sqref="F8:F12 A3"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1737,7 +1748,9 @@
       <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1752,6 +1765,9 @@
       </c>
       <c r="C3" t="s">
         <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1765,11 +1781,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView windowProtection="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCellId="1" sqref="F8:F12 A1"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1828,7 +1844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView windowProtection="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2223,7 +2239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView windowProtection="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2481,7 +2497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2515,7 +2531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView windowProtection="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2549,14 +2565,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView windowProtection="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D21" activeCellId="1" sqref="F8:F12 D21"/>
+      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.5" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -2682,7 +2709,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="105" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>103</v>
       </c>
@@ -2696,7 +2723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>105</v>
       </c>
@@ -2710,7 +2737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="105" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>107</v>
       </c>
@@ -2724,7 +2751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="105" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>109</v>
       </c>
@@ -2738,7 +2765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="105" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
refactoring for consistency with unittest framework; updating for updates to wc-sim (removal of cell_cycle_len and dry_weight parameters; ignoring wps temporary files
</commit_message>
<xml_diff>
--- a/tests/fixtures/min_model.xlsx
+++ b/tests/fixtures/min_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19800" windowHeight="6840" tabRatio="993" activeTab="1"/>
+    <workbookView windowWidth="19800" windowHeight="6840" tabRatio="993" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Rate laws'!$C$1:$K$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'dFBA net reactions'!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'dFBA net species'!$A$1:$G$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">Parameters!$A$1:$F$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">Parameters!$A$1:$F$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'Stop conditions'!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">References!$A$1:$Q$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="0">Model!$A$1:$B$8</definedName>
@@ -143,14 +143,14 @@
     <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="14">'dFBA net species'!$A$1:$G$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="14">'dFBA net species'!$A$1:$G$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="14">'dFBA net species'!$A$1:$G$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="15">Parameters!$A$1:$F$3</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="15">Parameters!$A$1:$F$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="15">Parameters!$A$1:$F$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$3</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="15">Parameters!$A$1:$F$2</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="15">Parameters!$A$1:$F$2</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="15">Parameters!$A$1:$F$2</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$2</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$2</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$2</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$2</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$2</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="16">'Stop conditions'!$A$1:$D$1</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="16">'Stop conditions'!$A$1:$D$1</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="16">'Stop conditions'!$A$1:$D$1</definedName>
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="230">
   <si>
     <t>Id</t>
   </si>
@@ -784,13 +784,7 @@
     <t>Standard error</t>
   </si>
   <si>
-    <t>cell_cycle_len</t>
-  </si>
-  <si>
-    <t>fractionDryWeight</t>
-  </si>
-  <si>
-    <t>dimensionless</t>
+    <t>mean_doubling_time</t>
   </si>
   <si>
     <t>k_cat</t>
@@ -877,9 +871,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -934,46 +928,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -988,7 +944,82 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1001,9 +1032,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1017,47 +1047,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1082,7 +1076,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1094,7 +1160,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1106,19 +1208,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1130,19 +1226,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1160,97 +1244,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1294,6 +1288,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1305,6 +1308,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1324,17 +1342,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1349,143 +1361,125 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1495,11 +1489,11 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2384,13 +2378,13 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="24.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.675" style="1"/>
+    <col min="2" max="2" width="5.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.625" style="1" customWidth="1"/>
     <col min="5" max="5" width="4.875" style="1" customWidth="1"/>
@@ -2827,14 +2821,14 @@
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14:F16"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2842,7 +2836,7 @@
     <col min="1" max="1" width="15.25" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.78333333333333" style="1"/>
     <col min="3" max="3" width="5.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.25" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.78333333333333" style="1"/>
     <col min="6" max="6" width="14.375" style="1" customWidth="1"/>
     <col min="7" max="1025" width="8.78333333333333" style="1"/>
@@ -2896,28 +2890,28 @@
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:6">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="D3" s="1">
-        <v>0.7</v>
+        <v>0.05</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>205</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D4" s="1">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>154</v>
@@ -2925,13 +2919,13 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D5" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>154</v>
@@ -2939,13 +2933,13 @@
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>154</v>
@@ -2953,13 +2947,13 @@
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D7" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>154</v>
@@ -2967,16 +2961,16 @@
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>186</v>
+        <v>205</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.035</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:6">
@@ -2984,115 +2978,101 @@
         <v>207</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D9" s="1">
         <v>0.035</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D10" s="1">
         <v>0.035</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" ht="15.1" customHeight="1" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0.035</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="12" ht="15.1" customHeight="1" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="13" ht="15.1" customHeight="1" spans="1:6">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>212</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>206</v>
+        <v>177</v>
       </c>
       <c r="D13" s="1">
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>177</v>
       </c>
       <c r="D14" s="1">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>212</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D15" s="1">
-        <v>1000</v>
+      <c r="D15" s="6">
+        <v>6.02214075862e+23</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D16" s="6">
-        <v>6.02214075862e+23</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:F16">
+  <autoFilter ref="A1:F15">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3190,19 +3170,19 @@
         <v>59</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>218</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>24</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>14</v>
@@ -3253,46 +3233,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>59</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>231</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>14</v>
@@ -3316,7 +3296,7 @@
   <sheetPr/>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -4329,17 +4309,17 @@
   <sheetPr/>
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="A$1:A$1048576"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="14.8833333333333" style="1"/>
+    <col min="1" max="1" width="19.625" style="1" customWidth="1"/>
     <col min="2" max="1025" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
@@ -4423,7 +4403,7 @@
         <v>49</v>
       </c>
       <c r="E4" s="1">
-        <v>1000</v>
+        <v>100000</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>102</v>

</xml_diff>